<commit_message>
add timesheet week 8
</commit_message>
<xml_diff>
--- a/Documentation/TimeSheets/week3/HuyNguyen_timesheet_wk3.xlsx
+++ b/Documentation/TimeSheets/week3/HuyNguyen_timesheet_wk3.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Adelaide\2017-S2-SEP-PG29\Documentation\TimeSheets\week3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\3. Adelaide - Source Code\2017-S2-SEP-PG29\Documentation\TimeSheets\week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,9 +62,6 @@
     <t>Client Meeting</t>
   </si>
   <si>
-    <t>Huy Nguyen</t>
-  </si>
-  <si>
     <t>Team Meeting Minute</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Self-leaning JavaUI to make UI control</t>
+  </si>
+  <si>
+    <t>Huy Nguyen Phan</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -488,7 +488,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -580,7 +580,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3">
         <v>42957</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3">
         <v>42958</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
         <v>42960</v>
@@ -634,7 +634,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" s="3">
         <v>42960</v>
@@ -694,7 +694,7 @@
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="4"/>

</xml_diff>